<commit_message>
Added diode 1N4007 to circuit
update to assembly protocol and purchase list to include diode 1N4007 in solenoid circuit.  Addition of diode should reduce solenoid disruption of Arduino serial connection.
</commit_message>
<xml_diff>
--- a/purchase_list.xlsx
+++ b/purchase_list.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Documents\GitHub\headfixed_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC874040-38B3-41BA-9663-C2AEFE2715CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12644C7-887C-4EA7-8CC8-F9525B4154F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43250" yWindow="3030" windowWidth="28800" windowHeight="15650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="164">
   <si>
     <t>item</t>
   </si>
@@ -514,6 +514,12 @@
   </si>
   <si>
     <t>1 for brake, 1 for retractable spout, 1 for radial spout</t>
+  </si>
+  <si>
+    <t>Diode 1N4007</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BOJACK-Rectifier-IN4007-Electronic-Silicon/dp/B07Q6J9TNW</t>
   </si>
 </sst>
 </file>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1634,51 +1640,51 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>85</v>
+      <c r="C30" s="1">
+        <v>125</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>15.8</v>
+        <v>5.99</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>13.88</v>
+        <v>15.8</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>159</v>
@@ -1686,62 +1692,62 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="D32" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>1.5</v>
+        <v>13.88</v>
       </c>
       <c r="F32" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>178.85</v>
+        <v>1.5</v>
       </c>
       <c r="F33" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -1750,47 +1756,47 @@
         <v>1</v>
       </c>
       <c r="E34" s="1">
-        <v>2</v>
+        <v>178.85</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="1">
-        <v>33.25</v>
-      </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>102</v>
@@ -1799,50 +1805,50 @@
         <v>25</v>
       </c>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1">
-        <v>53.5</v>
+        <v>33.25</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
       <c r="E37" s="1">
-        <v>9.99</v>
+        <v>53.5</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
@@ -1854,21 +1860,21 @@
         <v>1</v>
       </c>
       <c r="E38" s="1">
-        <v>8.2799999999999994</v>
+        <v>9.99</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
@@ -1880,21 +1886,21 @@
         <v>1</v>
       </c>
       <c r="E39" s="1">
-        <v>2.86</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
@@ -1906,47 +1912,47 @@
         <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>4.7699999999999996</v>
+        <v>2.86</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="1">
-        <v>11.95</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>120</v>
@@ -1955,16 +1961,16 @@
         <v>100</v>
       </c>
       <c r="D42" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1">
-        <v>6.45</v>
+        <v>11.95</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>115</v>
@@ -1972,7 +1978,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>120</v>
@@ -1981,16 +1987,16 @@
         <v>100</v>
       </c>
       <c r="D43" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E43" s="1">
-        <v>2.89</v>
+        <v>6.45</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>115</v>
@@ -1998,7 +2004,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>120</v>
@@ -2007,16 +2013,16 @@
         <v>100</v>
       </c>
       <c r="D44" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E44" s="1">
-        <v>1.18</v>
+        <v>2.89</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>115</v>
@@ -2024,7 +2030,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>120</v>
@@ -2036,13 +2042,13 @@
         <v>1</v>
       </c>
       <c r="E45" s="1">
-        <v>1.74</v>
+        <v>1.18</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>115</v>
@@ -2050,48 +2056,51 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="C46" s="1">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="D46" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1">
-        <v>10.99</v>
+        <v>1.74</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>134</v>
+        <v>5</v>
+      </c>
+      <c r="E47" s="1">
+        <v>10.99</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>159</v>
@@ -2099,129 +2108,126 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
       <c r="D48" s="1">
-        <v>4</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0.15</v>
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="F48" s="1">
-        <v>4</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E49" s="1">
-        <v>3.97</v>
+        <v>0.15</v>
       </c>
       <c r="F49" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="C50" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E50" s="1">
-        <v>24.63</v>
+        <v>3.97</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="C51" s="1">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D51" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E51" s="1">
-        <v>9.99</v>
+        <v>24.63</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D52" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1">
-        <v>20.97</v>
+        <v>9.99</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>159</v>
@@ -2229,84 +2235,110 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="1">
-        <v>1110</v>
+        <v>12</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
       </c>
       <c r="E53" s="1">
-        <v>20.010000000000002</v>
+        <v>20.97</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="1">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>153</v>
+        <v>1110</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
       </c>
       <c r="E54" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>153</v>
+        <v>20.010000000000002</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="1">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E55" s="1">
-        <v>13.95</v>
+        <v>12.99</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>153</v>
       </c>
       <c r="G55" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="1">
+        <v>25</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="1">
+        <v>13.95</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>158</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H56" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>